<commit_message>
updated Blocks documentation to include new command numbers to avoid sending '+' character to Bluetooth UART
</commit_message>
<xml_diff>
--- a/layouts/lightplay2a/lightplay2a-BillOfMaterials.xlsx
+++ b/layouts/lightplay2a/lightplay2a-BillOfMaterials.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
   <si>
     <t>10 uH inductor</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Arduino</t>
   </si>
   <si>
-    <t>Dc/Dc converter</t>
-  </si>
-  <si>
     <t>LT1615</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>SOT-23-3</t>
   </si>
   <si>
-    <t>785-1012-1-ND</t>
-  </si>
-  <si>
     <t>Distributor</t>
   </si>
   <si>
@@ -264,9 +258,6 @@
     <t>R0-R11</t>
   </si>
   <si>
-    <t>PPC5.6W-1CT-ND</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -288,9 +279,6 @@
     <t>0.1 uF cap</t>
   </si>
   <si>
-    <t>axial through hole</t>
-  </si>
-  <si>
     <t>R12</t>
   </si>
   <si>
@@ -303,9 +291,6 @@
     <t xml:space="preserve">1M </t>
   </si>
   <si>
-    <t>120k</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -318,15 +303,6 @@
     <t>10k</t>
   </si>
   <si>
-    <t>ERJ-6ENF1203V</t>
-  </si>
-  <si>
-    <t>667-ERJ-6ENF1203V</t>
-  </si>
-  <si>
-    <t>PR01000105608JR500</t>
-  </si>
-  <si>
     <t>CRCW08051M00FKEA</t>
   </si>
   <si>
@@ -363,53 +339,92 @@
     <t>621-DMN3150L-7</t>
   </si>
   <si>
-    <t>Diodes Inc</t>
-  </si>
-  <si>
     <t>alt:</t>
   </si>
   <si>
     <t>710-744025100</t>
   </si>
   <si>
-    <t>594-5073NW5R600J</t>
-  </si>
-  <si>
-    <t>soic</t>
-  </si>
-  <si>
-    <t>3.3Vreg</t>
-  </si>
-  <si>
     <t>L78L33ACD13TR</t>
   </si>
   <si>
-    <t>5.6 ohm 1 or 2  W resistors</t>
-  </si>
-  <si>
-    <t>284-ACS5SW-5.6</t>
-  </si>
-  <si>
-    <t>284-ACS5SW-8.2</t>
-  </si>
-  <si>
-    <t>R0, R4, R8</t>
-  </si>
-  <si>
-    <t>R1-R3, R5-R7, R9-R11</t>
-  </si>
-  <si>
-    <t>5W 5.6 ohm resistor</t>
-  </si>
-  <si>
-    <t>5W 8.2 ohm resistor</t>
+    <t>284-ACS5SW-6.8</t>
+  </si>
+  <si>
+    <t>ACS 5s 6R8 J T&amp;R</t>
+  </si>
+  <si>
+    <t>Ohmite/Arcol</t>
+  </si>
+  <si>
+    <t>throughhole</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5W 6.8 ohm wirewound resistor  </t>
+  </si>
+  <si>
+    <t>56k</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF5602V</t>
+  </si>
+  <si>
+    <t>667-ERJ-6ENF5602V</t>
+  </si>
+  <si>
+    <t>C4-C6</t>
+  </si>
+  <si>
+    <t>511-L78L33ACD-TR</t>
+  </si>
+  <si>
+    <t>soic8</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>0.33 uF cap</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>3.3V regulator</t>
+  </si>
+  <si>
+    <t>DC/DC converter</t>
+  </si>
+  <si>
+    <t>81-GRM40X104K50L</t>
+  </si>
+  <si>
+    <t>GRM21BR71H104KA01L</t>
+  </si>
+  <si>
+    <t>81-GRM40X334K16L</t>
+  </si>
+  <si>
+    <t>GRM21BR71C334KA01L</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>C1206</t>
+  </si>
+  <si>
+    <t>leave out, better to put on motor jack</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -482,24 +497,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -518,7 +515,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -718,8 +715,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -764,16 +785,8 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="223">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -894,6 +907,18 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
@@ -972,6 +997,18 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1304,7 +1341,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1325,34 +1362,34 @@
   <sheetData>
     <row r="1" spans="1:12" s="13" customFormat="1" ht="45">
       <c r="A1" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="12" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H1" s="14" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>11</v>
@@ -1361,7 +1398,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -1370,16 +1407,16 @@
         <v>744025100</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>116</v>
+        <v>18</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="H2" s="6">
         <v>1.5</v>
@@ -1394,12 +1431,12 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>1</v>
@@ -1417,16 +1454,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="6">
         <v>0.12</v>
@@ -1435,7 +1472,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J14" si="0">I4*H4</f>
+        <f t="shared" ref="J4:J13" si="0">I4*H4</f>
         <v>0.12</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -1444,22 +1481,22 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>6</v>
@@ -1477,25 +1514,25 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="F6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>113</v>
+        <v>18</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="H6" s="6">
         <v>0.2</v>
@@ -1508,232 +1545,247 @@
         <v>2.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
+    <row r="7" spans="1:12" ht="14" customHeight="1">
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>12</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:12" ht="14" customHeight="1">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H8" s="6">
-        <v>17.5</v>
+        <v>9.9499999999999993</v>
       </c>
       <c r="I8" s="17">
         <v>1</v>
       </c>
       <c r="J8" s="6">
         <f t="shared" si="0"/>
-        <v>17.5</v>
+        <v>9.9499999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:12">
+      <c r="A9" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>20</v>
+        <v>125</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H9" s="6">
-        <v>9.9499999999999993</v>
+        <v>3.35</v>
       </c>
       <c r="I9" s="17">
         <v>1</v>
       </c>
       <c r="J9" s="6">
         <f t="shared" si="0"/>
-        <v>9.9499999999999993</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>61</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
+        <v>80</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>26</v>
+        <v>51</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="H10" s="6">
-        <v>3.35</v>
+        <v>2.95</v>
       </c>
       <c r="I10" s="17">
         <v>1</v>
       </c>
       <c r="J10" s="6">
         <f t="shared" si="0"/>
-        <v>3.35</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>50</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>84</v>
+        <v>36</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="H11" s="6">
-        <v>2.95</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="I11" s="17">
         <v>1</v>
       </c>
       <c r="J11" s="6">
         <f t="shared" si="0"/>
-        <v>2.95</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>36</v>
+        <v>20</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="H12" s="6">
-        <v>1.1299999999999999</v>
+        <v>7.95</v>
       </c>
       <c r="I12" s="17">
         <v>1</v>
       </c>
       <c r="J12" s="6">
         <f t="shared" si="0"/>
-        <v>1.1299999999999999</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="B13" s="2" t="s">
-        <v>41</v>
+      <c r="A13" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="H13" s="6">
-        <v>7.95</v>
+        <v>1.5</v>
       </c>
       <c r="I13" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J13" s="6">
         <f t="shared" si="0"/>
-        <v>7.95</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="B14" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H14" s="6">
-        <v>1.5</v>
+        <v>0.35</v>
       </c>
       <c r="I14" s="17">
         <v>3</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f t="shared" ref="J14:J29" si="1">I14*H14</f>
+        <v>1.0499999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:12">
+      <c r="A15" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>47</v>
+        <v>18</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>53</v>
       </c>
       <c r="H15" s="6">
-        <v>0.35</v>
+        <v>0.89</v>
       </c>
       <c r="I15" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" ref="J15:J29" si="1">I15*H15</f>
-        <v>1.0499999999999998</v>
+        <f t="shared" si="1"/>
+        <v>0.89</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1743,411 +1795,417 @@
       <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="E16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>54</v>
+        <v>36</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="H16" s="6">
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
       <c r="I16" s="17">
         <v>1</v>
       </c>
       <c r="J16" s="6">
         <f t="shared" si="1"/>
-        <v>0.89</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>113</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="H17" s="6">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="I17" s="17">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" si="1"/>
-        <v>0.95</v>
+        <v>9.6000000000000014</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E18" s="25" t="s">
+      <c r="C18" s="9"/>
+      <c r="G18" s="11"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="C19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="H18" s="26">
-        <v>0.11</v>
-      </c>
-      <c r="I18" s="27">
-        <v>12</v>
-      </c>
-      <c r="J18" s="26"/>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="C19" s="9"/>
-      <c r="F19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" s="17"/>
+      <c r="G19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I19" s="17">
+        <v>1</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="1"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C20" s="9"/>
+        <v>114</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="F20" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" t="s">
-        <v>122</v>
+        <v>18</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="H20" s="6">
-        <v>0.8</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I20" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J20" s="6">
         <f t="shared" si="1"/>
-        <v>2.4000000000000004</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C21" s="9"/>
+        <v>90</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>88</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" t="s">
-        <v>123</v>
+        <v>18</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="H21" s="6">
-        <v>0.8</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="I21" s="17">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J21" s="6">
         <f t="shared" si="1"/>
-        <v>7.2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="C22" s="9"/>
-      <c r="G22" s="22"/>
-      <c r="I22" s="17"/>
+      <c r="A22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H22" s="6">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I22" s="17">
+        <v>3</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="1"/>
+        <v>8.4000000000000005E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>102</v>
+        <v>56</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>103</v>
+        <v>18</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>58</v>
       </c>
       <c r="H23" s="6">
-        <v>2.8000000000000001E-2</v>
+        <v>1.62</v>
       </c>
       <c r="I23" s="17">
         <v>1</v>
       </c>
       <c r="J23" s="6">
         <f t="shared" si="1"/>
-        <v>2.8000000000000001E-2</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="4" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>100</v>
+        <v>18</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>104</v>
       </c>
       <c r="H24" s="6">
-        <v>1.6E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="I24" s="17">
         <v>1</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" si="1"/>
-        <v>1.6E-2</v>
+        <v>5.6000000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="4" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>104</v>
+        <v>84</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>105</v>
+        <v>18</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="H25" s="6">
-        <v>2.8000000000000001E-2</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="I25" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="1"/>
-        <v>5.6000000000000001E-2</v>
+        <v>0.10199999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="4" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>107</v>
+        <v>85</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>127</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>106</v>
+        <v>18</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>126</v>
       </c>
       <c r="H26" s="6">
-        <v>2.8000000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="I26" s="17">
         <v>3</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>8.4000000000000005E-2</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="4" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E27" s="5">
-        <v>1206</v>
+      <c r="E27" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="H27" s="6">
-        <v>1.62</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="I27" s="17">
         <v>1</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" si="1"/>
-        <v>1.62</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
-        <v>85</v>
+        <v>123</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="5">
-        <v>1206</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="6">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="I28" s="17">
-        <v>1</v>
-      </c>
-      <c r="J28" s="6">
-        <f t="shared" si="1"/>
-        <v>5.6000000000000001E-2</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="G28" s="11"/>
+      <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>110</v>
+        <v>124</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="5">
-        <v>1206</v>
+        <v>51</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="H29" s="6">
-        <v>0.10199999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="I29" s="17">
         <v>1</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" si="1"/>
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="16">
-      <c r="B30" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="23" t="s">
-        <v>120</v>
-      </c>
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:10">
       <c r="G31" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" s="21">
-        <f>SUM(H2:H29)</f>
-        <v>53.447999999999993</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="H31" s="21"/>
       <c r="I31" s="21"/>
       <c r="J31" s="21">
-        <f>SUM(J2:J29)</f>
-        <v>67.322000000000017</v>
+        <f>SUM(J2:J25)</f>
+        <v>67.322000000000031</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed middle motor speed from 6/10 to 7/10
</commit_message>
<xml_diff>
--- a/layouts/lightplay2a/lightplay2a-BillOfMaterials.xlsx
+++ b/layouts/lightplay2a/lightplay2a-BillOfMaterials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="220" windowWidth="33900" windowHeight="22340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,9 +270,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>1.0 uF cap</t>
   </si>
   <si>
@@ -372,9 +369,6 @@
     <t>667-ERJ-6ENF5602V</t>
   </si>
   <si>
-    <t>C4-C6</t>
-  </si>
-  <si>
     <t>511-L78L33ACD-TR</t>
   </si>
   <si>
@@ -418,6 +412,12 @@
   </si>
   <si>
     <t>leave out, better to put on motor jack</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C3-C6</t>
   </si>
 </sst>
 </file>
@@ -515,7 +515,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="223">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -660,6 +660,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -786,7 +788,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="223">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -919,6 +921,7 @@
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
@@ -1009,6 +1012,7 @@
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1338,10 +1342,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1416,7 +1423,7 @@
         <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H2" s="6">
         <v>1.5</v>
@@ -1431,7 +1438,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="8"/>
       <c r="E3" s="8"/>
@@ -1532,7 +1539,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H6" s="6">
         <v>0.2</v>
@@ -1598,7 +1605,7 @@
         <v>62</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>14</v>
@@ -1820,22 +1827,22 @@
         <v>78</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H17" s="6">
         <v>0.8</v>
@@ -1855,25 +1862,25 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H19" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1888,25 +1895,25 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>115</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H20" s="6">
         <v>1.6E-2</v>
@@ -1921,25 +1928,25 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1954,25 +1961,25 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="C22" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="6">
         <v>2.8000000000000001E-2</v>
@@ -1999,7 +2006,7 @@
         <v>57</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>18</v>
@@ -2023,22 +2030,22 @@
         <v>82</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" s="6">
         <v>5.6000000000000001E-2</v>
@@ -2053,52 +2060,52 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="4" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>84</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G25" s="11" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="H25" s="6">
-        <v>0.10199999999999999</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="I25" s="17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" si="1"/>
-        <v>0.10199999999999999</v>
+        <v>0.126</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>127</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>18</v>
@@ -2107,14 +2114,14 @@
         <v>126</v>
       </c>
       <c r="H26" s="6">
-        <v>4.2000000000000003E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="I26" s="17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" si="1"/>
-        <v>0.126</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -2122,66 +2129,66 @@
         <v>121</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" s="6">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="I27" s="17">
-        <v>1</v>
-      </c>
-      <c r="J27" s="6">
-        <f t="shared" si="1"/>
-        <v>6.9000000000000006E-2</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="G27" s="11"/>
+      <c r="I27" s="17"/>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="4" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C28" s="9"/>
-      <c r="G28" s="11"/>
-      <c r="I28" s="17"/>
+        <v>83</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="I28" s="17">
+        <v>1</v>
+      </c>
+      <c r="J28" s="6">
+        <f>I28*H28</f>
+        <v>0.10199999999999999</v>
+      </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>51</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H29" s="6">
         <v>0.14000000000000001</v>
@@ -2204,17 +2211,17 @@
       <c r="H31" s="21"/>
       <c r="I31" s="21"/>
       <c r="J31" s="21">
-        <f>SUM(J2:J25)</f>
-        <v>67.322000000000031</v>
+        <f>SUM(J2:J28)</f>
+        <v>67.517000000000039</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="51" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>